<commit_message>
Modified project plan to draft version 1.0.
</commit_message>
<xml_diff>
--- a/iCozy_Project_Planning.xlsx
+++ b/iCozy_Project_Planning.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="97">
   <si>
     <t>Imagine Cup 2016 微软“创新杯”全球学生科技大赛</t>
   </si>
@@ -104,7 +104,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Microsoft YaHei"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>站点注册</t>
     </r>
@@ -369,22 +369,35 @@
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
+    <t>liuyinyu14ww@hotmail.com</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>luoshiwei14ww@hotmail.com</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>[世界公民]该作品具有很广的影响范围，所有采用大量点光源照明的场所都可以从本方案中受益。作品所解决的照明节能问题对于我们共同保护生态环境具有非常积极的意义。作品针对现有智能照明解决方案进行了一定程度的创新，主要体现在利用智能控制器本身的通信系统对使用者进行距离判定，既避免了精确定位带来的技术复杂性，又能达到期望的目的。</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>a) 这是一个典型的传感器网络系统，分为无线传感网、PC端（或云端）和用户端三大部分。目前的计划是：无线传感网采用TI的CC2530硬件平台及配套的ZStack；PC端（或云端）采用B/S架构，核心服务为HTTP服务，用微软的IIS实现；用户端使用Windows Mobile平台的APP。b) 无线传感网部分采用TI公司配套的IAR集成开发环境；PC端及用户端APP使用微软的VisualStudio开发环境和Windows 10 SDK。系统的运行环境分别为：传感网部分为ZStack，PC端及用户端为Windows。c)系统的功能只有一个：根据使用者的位置动态地调整环境光源的强度，使得距离使用者最近的光源强度最高。为了实现这个功能，需要PC端和APP端具备一定的辅助功能：PC端作为后端对传感网采集到的数据进行处理，和环境背景数据进行对比，用于分析不同光源强度应该如何分配，APP端用于向用户报告系统实时的数据并接收用户对系统的指令。</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>刘饮渝及罗世伟——负责1）PC端和APP的开发及网络搭建；2）传感网的集成测试；3）部分文档的撰写；许烙及李浩——负责 1）传感网部分的开发和硬件平台的搭建；2）PC端及APP的集成测试；3）视频制作及演示文档的撰写</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
     <t>qixuan98586@hotmail.com</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>liuyinyu14ww@hotmail.com</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>luoshiwei14ww@hotmail.com</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
     <t>lihao1996@hotmail.com</t>
-  </si>
-  <si>
-    <t>[世界公民]该作品具有很广的影响范围，所有采用大量点光源照明的场所都可以从本方案中受益。作品所解决的照明节能问题对于我们共同保护生态环境具有非常积极的意义。作品针对现有智能照明解决方案进行了一定程度的创新，主要体现在利用智能控制器本身的通信系统对使用者进行距离判定，既避免了精确定位带来的技术复杂性，又能达到期望的目的。</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>qixuan98586@hotmail.com</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -405,28 +418,28 @@
       <sz val="21.5"/>
       <color rgb="FF7030A0"/>
       <name val="Microsoft YaHei"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="22.5"/>
       <color rgb="FF7030A0"/>
       <name val="Microsoft YaHei"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Microsoft YaHei"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -439,7 +452,7 @@
       <sz val="10"/>
       <color rgb="FF7030A0"/>
       <name val="Microsoft YaHei"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -468,7 +481,7 @@
       <sz val="11"/>
       <color rgb="FF7030A0"/>
       <name val="Microsoft YaHei"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -819,7 +832,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -855,18 +868,93 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -888,12 +976,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -909,77 +991,9 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="2"/>
@@ -1024,7 +1038,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1453,8 +1467,8 @@
   </sheetPr>
   <dimension ref="B1:N72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55:F59"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1469,106 +1483,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="53.25" customHeight="1">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="2:12" ht="48" customHeight="1">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="2:12" ht="15">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="52"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="2:12" ht="16.5">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="2:12" ht="16.5">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="2:12" ht="16.5">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="2:12" ht="16.5">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
     </row>
     <row r="8" spans="2:12" ht="16.5">
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="19">
         <v>15085059763</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="2:12" ht="16.5">
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
+      <c r="C9" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="2:12" ht="16.5">
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
       <c r="L10" s="11" t="s">
         <v>10</v>
       </c>
@@ -1577,12 +1593,12 @@
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
       <c r="L11" s="11" t="s">
         <v>13</v>
       </c>
@@ -1591,12 +1607,12 @@
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="42"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="23"/>
       <c r="L12" s="11" t="s">
         <v>15</v>
       </c>
@@ -1605,30 +1621,30 @@
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
     </row>
     <row r="14" spans="2:12" ht="15">
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="46"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="2:12" ht="51" customHeight="1">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
     </row>
     <row r="16" spans="2:12" ht="17.25" thickBot="1">
       <c r="B16" s="4" t="s">
@@ -1651,78 +1667,78 @@
       <c r="B17" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="53" t="s">
+      <c r="D17" s="13" t="s">
         <v>85</v>
       </c>
       <c r="E17" s="7">
         <v>15085059763</v>
       </c>
-      <c r="F17" s="55" t="s">
-        <v>89</v>
+      <c r="F17" s="8" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="14.25" thickBot="1">
       <c r="B18" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="53" t="s">
+      <c r="C18" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="53" t="s">
+      <c r="D18" s="13" t="s">
         <v>85</v>
       </c>
       <c r="E18" s="7">
         <v>18984918807</v>
       </c>
-      <c r="F18" s="54" t="s">
-        <v>92</v>
+      <c r="F18" s="8" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="14.25" thickBot="1">
       <c r="B19" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="53" t="s">
+      <c r="D19" s="13" t="s">
         <v>86</v>
       </c>
       <c r="E19" s="7">
         <v>15906902153</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="14.25" thickBot="1">
       <c r="B20" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="53" t="s">
+      <c r="D20" s="13" t="s">
         <v>86</v>
       </c>
       <c r="E20" s="9">
         <v>13385102656</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="14.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
       <c r="B21" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="53" t="s">
+      <c r="D21" s="13" t="s">
         <v>87</v>
       </c>
       <c r="E21" s="7">
@@ -1733,442 +1749,420 @@
       </c>
     </row>
     <row r="22" spans="2:6" ht="15">
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="25"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="30"/>
     </row>
     <row r="23" spans="2:6" ht="20.25" customHeight="1">
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
     </row>
     <row r="24" spans="2:6" ht="48.75" customHeight="1">
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
     </row>
     <row r="25" spans="2:6" ht="16.5">
       <c r="B25" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="37"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="36"/>
     </row>
     <row r="26" spans="2:6" ht="16.5" customHeight="1">
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="16"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="39"/>
     </row>
     <row r="27" spans="2:6" ht="17.25" customHeight="1">
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="19"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="44"/>
     </row>
     <row r="28" spans="2:6" ht="15" customHeight="1">
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="19"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="44"/>
     </row>
     <row r="29" spans="2:6" ht="15" customHeight="1">
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="19"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="44"/>
     </row>
     <row r="30" spans="2:6" ht="15" customHeight="1">
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="19"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="44"/>
     </row>
     <row r="31" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="22"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="47"/>
     </row>
     <row r="32" spans="2:6" ht="15">
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
     </row>
     <row r="33" spans="2:6" ht="71.25" customHeight="1">
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
     </row>
     <row r="34" spans="2:6">
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="16"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="39"/>
     </row>
     <row r="35" spans="2:6">
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="19"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="44"/>
     </row>
     <row r="36" spans="2:6">
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="19"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="44"/>
     </row>
     <row r="37" spans="2:6">
-      <c r="B37" s="17"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="19"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="44"/>
     </row>
     <row r="38" spans="2:6">
-      <c r="B38" s="20"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="22"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="47"/>
     </row>
     <row r="39" spans="2:6" ht="15">
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
     </row>
     <row r="40" spans="2:6" ht="164.25" customHeight="1">
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
     </row>
     <row r="41" spans="2:6">
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="39"/>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" s="42"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="44"/>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43" s="42"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="44"/>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="42"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="44"/>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45" s="45"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="47"/>
+    </row>
+    <row r="46" spans="2:6" s="1" customFormat="1" ht="15">
+      <c r="B46" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+    </row>
+    <row r="47" spans="2:6" s="1" customFormat="1" ht="39.75" customHeight="1">
+      <c r="B47" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="B48" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="39"/>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49" s="42"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="44"/>
+    </row>
+    <row r="50" spans="2:6">
+      <c r="B50" s="42"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="44"/>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="B51" s="42"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="44"/>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52" s="45"/>
+      <c r="C52" s="46"/>
+      <c r="D52" s="46"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="47"/>
+    </row>
+    <row r="53" spans="2:6" s="1" customFormat="1" ht="15">
+      <c r="B53" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="32"/>
+    </row>
+    <row r="54" spans="2:6" s="1" customFormat="1" ht="51.75" customHeight="1">
+      <c r="B54" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="33"/>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="39"/>
+    </row>
+    <row r="56" spans="2:6">
+      <c r="B56" s="42"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="44"/>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="B57" s="42"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="44"/>
+    </row>
+    <row r="58" spans="2:6">
+      <c r="B58" s="42"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="44"/>
+    </row>
+    <row r="59" spans="2:6">
+      <c r="B59" s="45"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="46"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="47"/>
+    </row>
+    <row r="60" spans="2:6" ht="15">
+      <c r="B60" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32"/>
+    </row>
+    <row r="61" spans="2:6" ht="16.5">
+      <c r="B61" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" s="33"/>
+      <c r="D61" s="33"/>
+      <c r="E61" s="33"/>
+      <c r="F61" s="33"/>
+    </row>
+    <row r="62" spans="2:6">
+      <c r="B62" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="16"/>
-    </row>
-    <row r="42" spans="2:6">
-      <c r="B42" s="17"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="19"/>
-    </row>
-    <row r="43" spans="2:6">
-      <c r="B43" s="17"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="19"/>
-    </row>
-    <row r="44" spans="2:6">
-      <c r="B44" s="17"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="19"/>
-    </row>
-    <row r="45" spans="2:6">
-      <c r="B45" s="20"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="22"/>
-    </row>
-    <row r="46" spans="2:6" s="1" customFormat="1" ht="15">
-      <c r="B46" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" s="33"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="33"/>
-    </row>
-    <row r="47" spans="2:6" s="1" customFormat="1" ht="39.75" customHeight="1">
-      <c r="B47" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-    </row>
-    <row r="48" spans="2:6">
-      <c r="B48" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="16"/>
-    </row>
-    <row r="49" spans="2:6">
-      <c r="B49" s="17"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="19"/>
-    </row>
-    <row r="50" spans="2:6">
-      <c r="B50" s="17"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="19"/>
-    </row>
-    <row r="51" spans="2:6">
-      <c r="B51" s="17"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="19"/>
-    </row>
-    <row r="52" spans="2:6">
-      <c r="B52" s="20"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="22"/>
-    </row>
-    <row r="53" spans="2:6" s="1" customFormat="1" ht="15">
-      <c r="B53" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
-    </row>
-    <row r="54" spans="2:6" s="1" customFormat="1" ht="51.75" customHeight="1">
-      <c r="B54" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-    </row>
-    <row r="55" spans="2:6">
-      <c r="B55" s="14"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="16"/>
-    </row>
-    <row r="56" spans="2:6">
-      <c r="B56" s="17"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="19"/>
-    </row>
-    <row r="57" spans="2:6">
-      <c r="B57" s="17"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="19"/>
-    </row>
-    <row r="58" spans="2:6">
-      <c r="B58" s="17"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="19"/>
-    </row>
-    <row r="59" spans="2:6">
-      <c r="B59" s="20"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="21"/>
-      <c r="F59" s="22"/>
-    </row>
-    <row r="60" spans="2:6" ht="15">
-      <c r="B60" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C60" s="33"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="33"/>
-    </row>
-    <row r="61" spans="2:6" ht="16.5">
-      <c r="B61" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C61" s="31"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="31"/>
-      <c r="F61" s="31"/>
-    </row>
-    <row r="62" spans="2:6">
-      <c r="B62" s="14"/>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
-      <c r="E62" s="15"/>
-      <c r="F62" s="16"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="38"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="39"/>
     </row>
     <row r="63" spans="2:6">
-      <c r="B63" s="17"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="19"/>
+      <c r="B63" s="42"/>
+      <c r="C63" s="43"/>
+      <c r="D63" s="43"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="44"/>
     </row>
     <row r="64" spans="2:6">
-      <c r="B64" s="17"/>
-      <c r="C64" s="18"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="18"/>
-      <c r="F64" s="19"/>
+      <c r="B64" s="42"/>
+      <c r="C64" s="43"/>
+      <c r="D64" s="43"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="44"/>
     </row>
     <row r="65" spans="2:6">
-      <c r="B65" s="17"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="18"/>
-      <c r="F65" s="19"/>
+      <c r="B65" s="42"/>
+      <c r="C65" s="43"/>
+      <c r="D65" s="43"/>
+      <c r="E65" s="43"/>
+      <c r="F65" s="44"/>
     </row>
     <row r="66" spans="2:6">
-      <c r="B66" s="20"/>
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="22"/>
+      <c r="B66" s="45"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="47"/>
     </row>
     <row r="67" spans="2:6" ht="17.25" customHeight="1">
-      <c r="B67" s="23" t="s">
+      <c r="B67" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
-      <c r="E67" s="24"/>
-      <c r="F67" s="25"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="30"/>
     </row>
     <row r="68" spans="2:6" ht="173.25" customHeight="1">
-      <c r="B68" s="26" t="s">
+      <c r="B68" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C68" s="27"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="27"/>
-      <c r="F68" s="27"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="50"/>
+      <c r="E68" s="50"/>
+      <c r="F68" s="50"/>
     </row>
     <row r="69" spans="2:6" ht="342.75" customHeight="1">
-      <c r="B69" s="28" t="s">
+      <c r="B69" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
+      <c r="C69" s="51"/>
+      <c r="D69" s="51"/>
+      <c r="E69" s="51"/>
+      <c r="F69" s="51"/>
     </row>
     <row r="70" spans="2:6" ht="23.25" customHeight="1">
-      <c r="B70" s="29" t="s">
+      <c r="B70" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C70" s="29"/>
-      <c r="D70" s="29"/>
-      <c r="E70" s="29"/>
-      <c r="F70" s="29"/>
+      <c r="C70" s="52"/>
+      <c r="D70" s="52"/>
+      <c r="E70" s="52"/>
+      <c r="F70" s="52"/>
     </row>
     <row r="71" spans="2:6" ht="21.75" customHeight="1">
-      <c r="B71" s="30" t="s">
+      <c r="B71" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="C71" s="30"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="30"/>
-      <c r="F71" s="30"/>
+      <c r="C71" s="53"/>
+      <c r="D71" s="53"/>
+      <c r="E71" s="53"/>
+      <c r="F71" s="53"/>
     </row>
     <row r="72" spans="2:6" ht="27" customHeight="1">
-      <c r="B72" s="13" t="s">
+      <c r="B72" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
+      <c r="C72" s="40"/>
+      <c r="D72" s="40"/>
+      <c r="E72" s="40"/>
+      <c r="F72" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B46:F46"/>
     <mergeCell ref="B72:F72"/>
     <mergeCell ref="B41:F45"/>
     <mergeCell ref="B27:F31"/>
@@ -2185,9 +2179,35 @@
     <mergeCell ref="B53:F53"/>
     <mergeCell ref="B54:F54"/>
     <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:F13">
       <formula1>$L$10:$L$12</formula1>
     </dataValidation>
@@ -2197,10 +2217,11 @@
     <hyperlink ref="F17" r:id="rId2"/>
     <hyperlink ref="F19" r:id="rId3"/>
     <hyperlink ref="F20" r:id="rId4"/>
+    <hyperlink ref="C9" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-  <drawing r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -2372,9 +2393,9 @@
         <f>中国区项目计划书!C8</f>
         <v>15085059763</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="str">
         <f>中国区项目计划书!C9</f>
-        <v>0</v>
+        <v>qixuan98586@hotmail.com</v>
       </c>
       <c r="G2" t="str">
         <f>中国区项目计划书!C10</f>

</xml_diff>